<commit_message>
Sept. presentations Updated default presentations
</commit_message>
<xml_diff>
--- a/Agendas/201709 San Diego WGM FHIR Agenda.xlsx
+++ b/Agendas/201709 San Diego WGM FHIR Agenda.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lloyd\Documents\SVN\FHIR\documents\Agendas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lloyd\Documents\SVN\FHIR-documents\documents\Agendas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
@@ -670,7 +671,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23:F23"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,11 +1121,11 @@
       <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
New Orleans agenda, corrections to Payors presentation
</commit_message>
<xml_diff>
--- a/Agendas/201709 San Diego WGM FHIR Agenda.xlsx
+++ b/Agendas/201709 San Diego WGM FHIR Agenda.xlsx
@@ -196,9 +196,6 @@
 or FM?</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>FGB?</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>SD?</t>
+  </si>
+  <si>
+    <t>BRR</t>
   </si>
 </sst>
 </file>
@@ -265,7 +265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +284,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -297,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -324,6 +330,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -671,7 +683,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,16 +795,16 @@
         <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -843,7 +855,7 @@
         <v>30</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -868,10 +880,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>12</v>
@@ -948,13 +960,13 @@
         <v>38</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1034,7 +1046,7 @@
         <v>14</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1054,7 +1066,7 @@
         <v>51</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1082,7 +1094,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>27</v>
@@ -1091,24 +1103,24 @@
         <v>49</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1118,14 +1130,14 @@
       <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>14</v>
+      <c r="C27" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>57</v>
+      <c r="E27" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>20</v>

</xml_diff>